<commit_message>
20220306 Mutacao e Casamento
</commit_message>
<xml_diff>
--- a/Dados/Debug/Roleta_Debug.xlsx
+++ b/Dados/Debug/Roleta_Debug.xlsx
@@ -477,46 +477,46 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>81</v>
+        <v>27</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cromossoma 81</t>
+          <t>Cromossoma 27</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1210.969425651885</v>
+        <v>1274.138079106776</v>
       </c>
       <c r="D2" t="n">
         <v>13</v>
       </c>
       <c r="E2" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F2" t="n">
         <v>84</v>
       </c>
       <c r="G2" t="n">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H2" t="n">
-        <v>0.02010290774201268</v>
+        <v>0.01982901923533602</v>
       </c>
       <c r="I2" t="n">
-        <v>0.02010290774201268</v>
+        <v>0.01982901923533602</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cromossoma 13</t>
+          <t>Cromossoma 20</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1286.13897636173</v>
+        <v>1289.821375846529</v>
       </c>
       <c r="D3" t="n">
         <v>14</v>
@@ -525,2416 +525,2416 @@
         <v>82</v>
       </c>
       <c r="F3" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G3" t="n">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H3" t="n">
-        <v>0.01950460691635755</v>
+        <v>0.01947280930895274</v>
       </c>
       <c r="I3" t="n">
-        <v>0.03960751465837023</v>
+        <v>0.03930182854428876</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cromossoma 15</t>
+          <t>Cromossoma 76</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1321.329504750158</v>
+        <v>1298.491549808137</v>
       </c>
       <c r="D4" t="n">
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F4" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G4" t="n">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H4" t="n">
-        <v>0.01926528658609549</v>
+        <v>0.01935407266682498</v>
       </c>
       <c r="I4" t="n">
-        <v>0.05887280124446571</v>
+        <v>0.05865590121111375</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cromossoma 80</t>
+          <t>Cromossoma 73</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1354.516303127823</v>
+        <v>1312.992728038412</v>
       </c>
       <c r="D5" t="n">
         <v>14</v>
       </c>
       <c r="E5" t="n">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F5" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G5" t="n">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0184276654301783</v>
+        <v>0.01911659938256946</v>
       </c>
       <c r="I5" t="n">
-        <v>0.07730046667464401</v>
+        <v>0.07777250059368321</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>12</v>
+        <v>66</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Cromossoma 12</t>
+          <t>Cromossoma 66</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1360.366874816026</v>
+        <v>1317.592657426874</v>
       </c>
       <c r="D6" t="n">
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="F6" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G6" t="n">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="H6" t="n">
-        <v>0.01794902476965418</v>
+        <v>0.01887912609831394</v>
       </c>
       <c r="I6" t="n">
-        <v>0.09524949144429819</v>
+        <v>0.09665162669199714</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cromossoma 4</t>
+          <t>Cromossoma 32</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1360.40739994667</v>
+        <v>1323.183782516269</v>
       </c>
       <c r="D7" t="n">
         <v>14</v>
       </c>
       <c r="E7" t="n">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="F7" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G7" t="n">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="H7" t="n">
-        <v>0.01782936460452315</v>
+        <v>0.01876038945618618</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1130788560488213</v>
+        <v>0.1154120161481833</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cromossoma 30</t>
+          <t>Cromossoma 71</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1370.24911376453</v>
+        <v>1326.315003969986</v>
       </c>
       <c r="D8" t="n">
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="F8" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G8" t="n">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="H8" t="n">
-        <v>0.01735072394399904</v>
+        <v>0.01852291617193066</v>
       </c>
       <c r="I8" t="n">
-        <v>0.1304295799928204</v>
+        <v>0.133934932320114</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cromossoma 61</t>
+          <t>Cromossoma 55</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1252.547642244188</v>
+        <v>1328.400187857577</v>
       </c>
       <c r="D9" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" t="n">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F9" t="n">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="G9" t="n">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="H9" t="n">
-        <v>0.01723106377886802</v>
+        <v>0.0184041795298029</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1476606437716884</v>
+        <v>0.1523391118499169</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Cromossoma 1</t>
+          <t>Cromossoma 46</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1292.972466746348</v>
+        <v>1329.168385291661</v>
       </c>
       <c r="D10" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E10" t="n">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="F10" t="n">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="G10" t="n">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="H10" t="n">
-        <v>0.01699174344860596</v>
+        <v>0.01816670624554738</v>
       </c>
       <c r="I10" t="n">
-        <v>0.1646523872202944</v>
+        <v>0.1705058180954642</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Cromossoma 32</t>
+          <t>Cromossoma 63</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1322.277595003258</v>
+        <v>1331.135091776353</v>
       </c>
       <c r="D11" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F11" t="n">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="G11" t="n">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0167524231183439</v>
+        <v>0.01804796960341962</v>
       </c>
       <c r="I11" t="n">
-        <v>0.1814048103386383</v>
+        <v>0.1885537876988838</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Cromossoma 51</t>
+          <t>Cromossoma 42</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1377.10959417888</v>
+        <v>1355.283624067468</v>
       </c>
       <c r="D12" t="n">
         <v>14</v>
       </c>
       <c r="E12" t="n">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F12" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G12" t="n">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0167524231183439</v>
+        <v>0.01745428639278081</v>
       </c>
       <c r="I12" t="n">
-        <v>0.1981572334569822</v>
+        <v>0.2060080740916647</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Cromossoma 15</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1366.213466823842</v>
+      </c>
+      <c r="D13" t="n">
+        <v>14</v>
+      </c>
+      <c r="E13" t="n">
         <v>63</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Cromossoma 63</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>1326.786052625302</v>
-      </c>
-      <c r="D13" t="n">
-        <v>15</v>
-      </c>
-      <c r="E13" t="n">
-        <v>78</v>
-      </c>
       <c r="F13" t="n">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="G13" t="n">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="H13" t="n">
-        <v>0.01663276295321288</v>
+        <v>0.01721681310852529</v>
       </c>
       <c r="I13" t="n">
-        <v>0.2147899964101951</v>
+        <v>0.22322488720019</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Cromossoma 31</t>
+          <t>Cromossoma 61</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1385.056711460949</v>
+        <v>1373.557959850644</v>
       </c>
       <c r="D14" t="n">
         <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F14" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G14" t="n">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="H14" t="n">
-        <v>0.01651310278808185</v>
+        <v>0.01686060318214201</v>
       </c>
       <c r="I14" t="n">
-        <v>0.2313030991982769</v>
+        <v>0.240085490382332</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Cromossoma 66</t>
+          <t>Cromossoma 72</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1386.804479398322</v>
+        <v>1375.170545784702</v>
       </c>
       <c r="D15" t="n">
         <v>14</v>
       </c>
       <c r="E15" t="n">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F15" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G15" t="n">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="H15" t="n">
-        <v>0.01627378245781979</v>
+        <v>0.01662312989788649</v>
       </c>
       <c r="I15" t="n">
-        <v>0.2475768816560967</v>
+        <v>0.2567086202802185</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Cromossoma 10</t>
+          <t>Cromossoma 2</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1332.110597778957</v>
+        <v>1219.115686002281</v>
       </c>
       <c r="D16" t="n">
         <v>15</v>
       </c>
       <c r="E16" t="n">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="F16" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G16" t="n">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H16" t="n">
-        <v>0.01627378245781979</v>
+        <v>0.01626691997150321</v>
       </c>
       <c r="I16" t="n">
-        <v>0.2638506641139165</v>
+        <v>0.2729755402517217</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Cromossoma 34</t>
+          <t>Cromossoma 64</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1391.679149642244</v>
+        <v>1393.934676759194</v>
       </c>
       <c r="D17" t="n">
         <v>14</v>
       </c>
       <c r="E17" t="n">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F17" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G17" t="n">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H17" t="n">
-        <v>0.01615412229268877</v>
+        <v>0.01591071004511992</v>
       </c>
       <c r="I17" t="n">
-        <v>0.2800047864066053</v>
+        <v>0.2888862502968416</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Cromossoma 44</t>
+          <t>Cromossoma 80</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1350.781322093577</v>
+        <v>1304.785704692375</v>
       </c>
       <c r="D18" t="n">
         <v>15</v>
       </c>
       <c r="E18" t="n">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F18" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G18" t="n">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H18" t="n">
-        <v>0.01615412229268877</v>
+        <v>0.01579197340299216</v>
       </c>
       <c r="I18" t="n">
-        <v>0.296158908699294</v>
+        <v>0.3046782236998337</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Cromossoma 47</t>
+          <t>Cromossoma 19</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1399.167094751029</v>
+        <v>1396.068264573718</v>
       </c>
       <c r="D19" t="n">
         <v>14</v>
       </c>
       <c r="E19" t="n">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F19" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G19" t="n">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H19" t="n">
-        <v>0.01591480196242671</v>
+        <v>0.0156732367608644</v>
       </c>
       <c r="I19" t="n">
-        <v>0.3120737106617207</v>
+        <v>0.3203514604606981</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Cromossoma 35</t>
+          <t>Cromossoma 69</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1357.681127550906</v>
+        <v>1315.680295134722</v>
       </c>
       <c r="D20" t="n">
         <v>15</v>
       </c>
       <c r="E20" t="n">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="F20" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G20" t="n">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H20" t="n">
-        <v>0.01579514179729568</v>
+        <v>0.01555450011873664</v>
       </c>
       <c r="I20" t="n">
-        <v>0.3278688524590164</v>
+        <v>0.3359059605794348</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Cromossoma 77</t>
+          <t>Cromossoma 43</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1409.330263148135</v>
+        <v>1329.16020944486</v>
       </c>
       <c r="D21" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E21" t="n">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="F21" t="n">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="G21" t="n">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="H21" t="n">
-        <v>0.01579514179729568</v>
+        <v>0.01484208026597008</v>
       </c>
       <c r="I21" t="n">
-        <v>0.3436639942563121</v>
+        <v>0.3507480408454048</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Cromossoma 2</t>
+          <t>Cromossoma 54</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1359.917077606149</v>
+        <v>1336.70653841647</v>
       </c>
       <c r="D22" t="n">
         <v>15</v>
       </c>
       <c r="E22" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F22" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G22" t="n">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="H22" t="n">
-        <v>0.01567548163216465</v>
+        <v>0.0144858703395868</v>
       </c>
       <c r="I22" t="n">
-        <v>0.3593394758884768</v>
+        <v>0.3652339111849917</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Cromossoma 67</t>
+          <t>Cromossoma 81</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1410.827146257315</v>
+        <v>1420.794243822951</v>
       </c>
       <c r="D23" t="n">
         <v>14</v>
       </c>
       <c r="E23" t="n">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F23" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G23" t="n">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H23" t="n">
-        <v>0.01531650113677157</v>
+        <v>0.0144858703395868</v>
       </c>
       <c r="I23" t="n">
-        <v>0.3746559770252483</v>
+        <v>0.3797197815245785</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Cromossoma 56</t>
+          <t>Cromossoma 58</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1365.143368715184</v>
+        <v>1342.12041311136</v>
       </c>
       <c r="D24" t="n">
         <v>15</v>
       </c>
       <c r="E24" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F24" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G24" t="n">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H24" t="n">
-        <v>0.01531650113677157</v>
+        <v>0.01436713369745904</v>
       </c>
       <c r="I24" t="n">
-        <v>0.3899724781620199</v>
+        <v>0.3940869152220375</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Cromossoma 48</t>
+          <t>Cromossoma 39</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1368.08592616006</v>
+        <v>1342.140751113044</v>
       </c>
       <c r="D25" t="n">
         <v>15</v>
       </c>
       <c r="E25" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F25" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G25" t="n">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="H25" t="n">
-        <v>0.01519684097164054</v>
+        <v>0.01424839705533128</v>
       </c>
       <c r="I25" t="n">
-        <v>0.4051693191336604</v>
+        <v>0.4083353122773687</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Cromossoma 0</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>1431.551970027032</v>
+      </c>
+      <c r="D26" t="n">
+        <v>14</v>
+      </c>
+      <c r="E26" t="n">
         <v>37</v>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Cromossoma 37</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>1370.88332061588</v>
-      </c>
-      <c r="D26" t="n">
-        <v>15</v>
-      </c>
-      <c r="E26" t="n">
-        <v>63</v>
-      </c>
       <c r="F26" t="n">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="G26" t="n">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="H26" t="n">
-        <v>0.01483786047624746</v>
+        <v>0.01412966041320352</v>
       </c>
       <c r="I26" t="n">
-        <v>0.4200071796099079</v>
+        <v>0.4224649726905723</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Cromossoma 68</t>
+          <t>Cromossoma 29</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1374.173927204964</v>
+        <v>1347.838120183805</v>
       </c>
       <c r="D27" t="n">
         <v>15</v>
       </c>
       <c r="E27" t="n">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F27" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G27" t="n">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="H27" t="n">
-        <v>0.0145985401459854</v>
+        <v>0.01412966041320352</v>
       </c>
       <c r="I27" t="n">
-        <v>0.4346057197558933</v>
+        <v>0.4365946331037758</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Cromossoma 50</t>
+          <t>Cromossoma 17</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1375.860344211297</v>
+        <v>1443.429500943633</v>
       </c>
       <c r="D28" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E28" t="n">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="F28" t="n">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="G28" t="n">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H28" t="n">
-        <v>0.01447887998085437</v>
+        <v>0.01401092377107575</v>
       </c>
       <c r="I28" t="n">
-        <v>0.4490845997367477</v>
+        <v>0.4506055568748515</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Cromossoma 19</t>
+          <t>Cromossoma 38</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1440.922263065247</v>
+        <v>1358.001591654587</v>
       </c>
       <c r="D29" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E29" t="n">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="F29" t="n">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="G29" t="n">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H29" t="n">
-        <v>0.01411989948546129</v>
+        <v>0.01389218712894799</v>
       </c>
       <c r="I29" t="n">
-        <v>0.463204499222209</v>
+        <v>0.4644977440037996</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Cromossoma 58</t>
+          <t>Cromossoma 18</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1385.653475561501</v>
+        <v>1445.511834719134</v>
       </c>
       <c r="D30" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E30" t="n">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="F30" t="n">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="G30" t="n">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H30" t="n">
-        <v>0.01400023932033026</v>
+        <v>0.01377345048682023</v>
       </c>
       <c r="I30" t="n">
-        <v>0.4772047385425393</v>
+        <v>0.4782711944906198</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Cromossoma 72</t>
+          <t>Cromossoma 56</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1397.902482825443</v>
+        <v>1366.481469601747</v>
       </c>
       <c r="D31" t="n">
         <v>15</v>
       </c>
       <c r="E31" t="n">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="F31" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G31" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H31" t="n">
-        <v>0.01364125882493718</v>
+        <v>0.01365471384469247</v>
       </c>
       <c r="I31" t="n">
-        <v>0.4908459973674764</v>
+        <v>0.4919259083353122</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Cromossoma 9</t>
+          <t>Cromossoma 74</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1402.074855839972</v>
+        <v>1373.430902126607</v>
       </c>
       <c r="D32" t="n">
         <v>15</v>
       </c>
       <c r="E32" t="n">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="F32" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G32" t="n">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H32" t="n">
-        <v>0.01340193849467512</v>
+        <v>0.01353597720256471</v>
       </c>
       <c r="I32" t="n">
-        <v>0.5042479358621516</v>
+        <v>0.505461885537877</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Cromossoma 52</t>
+          <t>Cromossoma 26</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1408.904858587838</v>
+        <v>1456.429924196272</v>
       </c>
       <c r="D33" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E33" t="n">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="F33" t="n">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="G33" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H33" t="n">
-        <v>0.01316261816441307</v>
+        <v>0.01329850391830919</v>
       </c>
       <c r="I33" t="n">
-        <v>0.5174105540265647</v>
+        <v>0.5187603894561862</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Cromossoma 7</t>
+          <t>Cromossoma 51</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1449.050756614643</v>
+        <v>1374.661890398213</v>
       </c>
       <c r="D34" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E34" t="n">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="F34" t="n">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="G34" t="n">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H34" t="n">
-        <v>0.01304295799928204</v>
+        <v>0.01329850391830919</v>
       </c>
       <c r="I34" t="n">
-        <v>0.5304535120258467</v>
+        <v>0.5320588933744954</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Cromossoma 70</t>
+          <t>Cromossoma 6</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1449.656256150245</v>
+        <v>1379.736141179391</v>
       </c>
       <c r="D35" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E35" t="n">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="F35" t="n">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="G35" t="n">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H35" t="n">
-        <v>0.01292329783415101</v>
+        <v>0.01306103063405367</v>
       </c>
       <c r="I35" t="n">
-        <v>0.5433768098599977</v>
+        <v>0.545119924008549</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Cromossoma 22</t>
+          <t>Cromossoma 70</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1419.239248866766</v>
+        <v>1463.50953125514</v>
       </c>
       <c r="D36" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E36" t="n">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="F36" t="n">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="G36" t="n">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="H36" t="n">
-        <v>0.01268397750388896</v>
+        <v>0.01294229399192591</v>
       </c>
       <c r="I36" t="n">
-        <v>0.5560607873638866</v>
+        <v>0.558062218000475</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Cromossoma 65</t>
+          <t>Cromossoma 31</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1419.32343947061</v>
+        <v>1381.765165742312</v>
       </c>
       <c r="D37" t="n">
         <v>15</v>
       </c>
       <c r="E37" t="n">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="F37" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G37" t="n">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="H37" t="n">
-        <v>0.01256431733875793</v>
+        <v>0.01294229399192591</v>
       </c>
       <c r="I37" t="n">
-        <v>0.5686251047026446</v>
+        <v>0.5710045119924009</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Cromossoma 40</t>
+          <t>Cromossoma 59</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1419.690872917478</v>
+        <v>1392.17395175611</v>
       </c>
       <c r="D38" t="n">
         <v>15</v>
       </c>
       <c r="E38" t="n">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F38" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G38" t="n">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="H38" t="n">
-        <v>0.0124446571736269</v>
+        <v>0.01282355734979815</v>
       </c>
       <c r="I38" t="n">
-        <v>0.5810697618762715</v>
+        <v>0.583828069342199</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Cromossoma 38</t>
+          <t>Cromossoma 67</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1422.191766797126</v>
+        <v>1464.088146353392</v>
       </c>
       <c r="D39" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E39" t="n">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="F39" t="n">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="G39" t="n">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="H39" t="n">
-        <v>0.01232499700849587</v>
+        <v>0.01282355734979815</v>
       </c>
       <c r="I39" t="n">
-        <v>0.5933947588847673</v>
+        <v>0.5966516266919971</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Cromossoma 0</t>
+          <t>Cromossoma 24</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1422.322139343242</v>
+        <v>1465.142367725736</v>
       </c>
       <c r="D40" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E40" t="n">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F40" t="n">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="G40" t="n">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="H40" t="n">
-        <v>0.01220533684336484</v>
+        <v>0.01270482070767039</v>
       </c>
       <c r="I40" t="n">
-        <v>0.6056000957281322</v>
+        <v>0.6093564473996675</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Cromossoma 39</t>
+          <t>Cromossoma 8</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1423.739194600314</v>
+        <v>1392.88831978238</v>
       </c>
       <c r="D41" t="n">
         <v>15</v>
       </c>
       <c r="E41" t="n">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="F41" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G41" t="n">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="H41" t="n">
-        <v>0.01208567667823382</v>
+        <v>0.01270482070767039</v>
       </c>
       <c r="I41" t="n">
-        <v>0.617685772406366</v>
+        <v>0.622061268107338</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Cromossoma 64</t>
+          <t>Cromossoma 62</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1463.527868333379</v>
+        <v>1393.154581583152</v>
       </c>
       <c r="D42" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E42" t="n">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="F42" t="n">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="G42" t="n">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="H42" t="n">
-        <v>0.01208567667823382</v>
+        <v>0.01258608406554263</v>
       </c>
       <c r="I42" t="n">
-        <v>0.6297714490845998</v>
+        <v>0.6346473521728806</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Cromossoma 14</t>
+          <t>Cromossoma 44</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1425.846409313839</v>
+        <v>1465.819269554238</v>
       </c>
       <c r="D43" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E43" t="n">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F43" t="n">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="G43" t="n">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="H43" t="n">
-        <v>0.01196601651310279</v>
+        <v>0.01246734742341487</v>
       </c>
       <c r="I43" t="n">
-        <v>0.6417374655977026</v>
+        <v>0.6471146995962954</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Cromossoma 36</t>
+          <t>Cromossoma 68</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1432.737244033526</v>
+        <v>1466.40997225413</v>
       </c>
       <c r="D44" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E44" t="n">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="F44" t="n">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="G44" t="n">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="H44" t="n">
-        <v>0.01172669618284073</v>
+        <v>0.01234861078128711</v>
       </c>
       <c r="I44" t="n">
-        <v>0.6534641617805433</v>
+        <v>0.6594633103775825</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Cromossoma 33</t>
+          <t>Cromossoma 22</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1473.157343681324</v>
+        <v>1395.727396701862</v>
       </c>
       <c r="D45" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E45" t="n">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="F45" t="n">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="G45" t="n">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="H45" t="n">
-        <v>0.01172669618284073</v>
+        <v>0.01234861078128711</v>
       </c>
       <c r="I45" t="n">
-        <v>0.6651908579633841</v>
+        <v>0.6718119211588697</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Cromossoma 5</t>
+          <t>Cromossoma 30</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1473.959259581011</v>
+        <v>1467.669918638915</v>
       </c>
       <c r="D46" t="n">
         <v>14</v>
       </c>
       <c r="E46" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F46" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G46" t="n">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="H46" t="n">
-        <v>0.0116070360177097</v>
+        <v>0.01222987413915934</v>
       </c>
       <c r="I46" t="n">
-        <v>0.6767978939810938</v>
+        <v>0.684041795298029</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Cromossoma 75</t>
+          <t>Cromossoma 77</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>1439.005497034725</v>
+        <v>1396.25459828313</v>
       </c>
       <c r="D47" t="n">
         <v>15</v>
       </c>
       <c r="E47" t="n">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F47" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G47" t="n">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="H47" t="n">
-        <v>0.0116070360177097</v>
+        <v>0.01211113749703158</v>
       </c>
       <c r="I47" t="n">
-        <v>0.6884049299988035</v>
+        <v>0.6961529327950606</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Cromossoma 17</t>
+          <t>Cromossoma 11</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1475.790888522613</v>
+        <v>1472.699618233064</v>
       </c>
       <c r="D48" t="n">
         <v>14</v>
       </c>
       <c r="E48" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F48" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="G48" t="n">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="H48" t="n">
-        <v>0.01148737585257868</v>
+        <v>0.01211113749703158</v>
       </c>
       <c r="I48" t="n">
-        <v>0.6998923058513822</v>
+        <v>0.7082640702920923</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Cromossoma 46</t>
+          <t>Cromossoma 21</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1440.636150637372</v>
+        <v>1399.525070977958</v>
       </c>
       <c r="D49" t="n">
         <v>15</v>
       </c>
       <c r="E49" t="n">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="F49" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G49" t="n">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="H49" t="n">
-        <v>0.01148737585257868</v>
+        <v>0.01199240085490382</v>
       </c>
       <c r="I49" t="n">
-        <v>0.7113796817039608</v>
+        <v>0.7202564711469961</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Cromossoma 25</t>
+          <t>Cromossoma 45</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1327.882375050367</v>
+        <v>1472.836326682917</v>
       </c>
       <c r="D50" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E50" t="n">
-        <v>77</v>
+        <v>19</v>
       </c>
       <c r="F50" t="n">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="G50" t="n">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="H50" t="n">
-        <v>0.01136771568744765</v>
+        <v>0.01199240085490382</v>
       </c>
       <c r="I50" t="n">
-        <v>0.7227473973914085</v>
+        <v>0.7322488720018999</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Cromossoma 53</t>
+          <t>Cromossoma 34</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1332.042108203029</v>
+        <v>1401.043540819189</v>
       </c>
       <c r="D51" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E51" t="n">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="F51" t="n">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="G51" t="n">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="H51" t="n">
-        <v>0.01124805552231662</v>
+        <v>0.01187366421277606</v>
       </c>
       <c r="I51" t="n">
-        <v>0.7339954529137251</v>
+        <v>0.7441225362146759</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>82</v>
+        <v>4</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Cromossoma 82</t>
+          <t>Cromossoma 4</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1441.621763271443</v>
+        <v>1401.401526326512</v>
       </c>
       <c r="D52" t="n">
         <v>15</v>
       </c>
       <c r="E52" t="n">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="F52" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G52" t="n">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="H52" t="n">
-        <v>0.01124805552231662</v>
+        <v>0.0117549275706483</v>
       </c>
       <c r="I52" t="n">
-        <v>0.7452435084360418</v>
+        <v>0.7558774637853243</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Cromossoma 59</t>
+          <t>Cromossoma 12</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1441.726187569202</v>
+        <v>1407.035774235464</v>
       </c>
       <c r="D53" t="n">
         <v>15</v>
       </c>
       <c r="E53" t="n">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="F53" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G53" t="n">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="H53" t="n">
-        <v>0.01112839535718559</v>
+        <v>0.01151745428639278</v>
       </c>
       <c r="I53" t="n">
-        <v>0.7563719037932274</v>
+        <v>0.767394918071717</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Cromossoma 69</t>
+          <t>Cromossoma 48</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1442.567327464099</v>
+        <v>1419.302947709967</v>
       </c>
       <c r="D54" t="n">
         <v>15</v>
       </c>
       <c r="E54" t="n">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="F54" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G54" t="n">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="H54" t="n">
-        <v>0.01088907502692354</v>
+        <v>0.01127998100213726</v>
       </c>
       <c r="I54" t="n">
-        <v>0.7672609788201509</v>
+        <v>0.7786748990738542</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Cromossoma 18</t>
+          <t>Cromossoma 50</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1446.566035586098</v>
+        <v>1420.737377818827</v>
       </c>
       <c r="D55" t="n">
         <v>15</v>
       </c>
       <c r="E55" t="n">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="F55" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G55" t="n">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="H55" t="n">
-        <v>0.01076941486179251</v>
+        <v>0.0111612443600095</v>
       </c>
       <c r="I55" t="n">
-        <v>0.7780303936819434</v>
+        <v>0.7898361434338638</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Cromossoma 3</t>
+          <t>Cromossoma 75</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>1503.101208199024</v>
+        <v>1424.434302641542</v>
       </c>
       <c r="D56" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E56" t="n">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="F56" t="n">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="G56" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H56" t="n">
-        <v>0.01076941486179251</v>
+        <v>0.01092377107575398</v>
       </c>
       <c r="I56" t="n">
-        <v>0.7887998085437359</v>
+        <v>0.8007599145096177</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>71</v>
+        <v>3</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Cromossoma 71</t>
+          <t>Cromossoma 3</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>1356.707050772633</v>
+        <v>1425.602088900844</v>
       </c>
       <c r="D57" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E57" t="n">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="F57" t="n">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="G57" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H57" t="n">
-        <v>0.01076941486179251</v>
+        <v>0.01080503443362622</v>
       </c>
       <c r="I57" t="n">
-        <v>0.7995692234055284</v>
+        <v>0.8115649489432439</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Cromossoma 54</t>
+          <t>Cromossoma 78</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1449.690137374204</v>
+        <v>1444.50221818695</v>
       </c>
       <c r="D58" t="n">
         <v>15</v>
       </c>
       <c r="E58" t="n">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F58" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G58" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H58" t="n">
-        <v>0.01041043436639943</v>
+        <v>0.01044882450724294</v>
       </c>
       <c r="I58" t="n">
-        <v>0.8099796577719278</v>
+        <v>0.8220137734504869</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Cromossoma 45</t>
+          <t>Cromossoma 35</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1450.472575140541</v>
+        <v>1324.770254663571</v>
       </c>
       <c r="D59" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E59" t="n">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="F59" t="n">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="G59" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H59" t="n">
-        <v>0.01017111403613737</v>
+        <v>0.01033008786511517</v>
       </c>
       <c r="I59" t="n">
-        <v>0.8201507718080652</v>
+        <v>0.832343861315602</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Cromossoma 28</t>
+          <t>Cromossoma 41</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1563.648349982609</v>
+        <v>1446.416522553136</v>
       </c>
       <c r="D60" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E60" t="n">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="F60" t="n">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="G60" t="n">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H60" t="n">
-        <v>0.009931793705875314</v>
+        <v>0.01021135122298741</v>
       </c>
       <c r="I60" t="n">
-        <v>0.8300825655139404</v>
+        <v>0.8425552125385894</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Cromossoma 21</t>
+          <t>Cromossoma 47</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>1453.944073963614</v>
+        <v>1543.98454248645</v>
       </c>
       <c r="D61" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E61" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="F61" t="n">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="G61" t="n">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H61" t="n">
-        <v>0.009931793705875314</v>
+        <v>0.01021135122298741</v>
       </c>
       <c r="I61" t="n">
-        <v>0.8400143592198157</v>
+        <v>0.8527665637615769</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Cromossoma 42</t>
+          <t>Cromossoma 57</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1369.940210178644</v>
+        <v>1576.051886132532</v>
       </c>
       <c r="D62" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E62" t="n">
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="F62" t="n">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="G62" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H62" t="n">
-        <v>0.009931793705875314</v>
+        <v>0.01009261458085965</v>
       </c>
       <c r="I62" t="n">
-        <v>0.849946152925691</v>
+        <v>0.8628591783424365</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Cromossoma 6</t>
+          <t>Cromossoma 25</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1454.904760856622</v>
+        <v>1451.940701212848</v>
       </c>
       <c r="D63" t="n">
         <v>15</v>
       </c>
       <c r="E63" t="n">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="F63" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G63" t="n">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H63" t="n">
-        <v>0.009812133540744287</v>
+        <v>0.01009261458085965</v>
       </c>
       <c r="I63" t="n">
-        <v>0.8597582864664353</v>
+        <v>0.8729517929232962</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Cromossoma 43</t>
+          <t>Cromossoma 23</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1468.920717876991</v>
+        <v>1452.170452822063</v>
       </c>
       <c r="D64" t="n">
         <v>15</v>
       </c>
       <c r="E64" t="n">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="F64" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G64" t="n">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="H64" t="n">
-        <v>0.00957281321048223</v>
+        <v>0.009973877938731893</v>
       </c>
       <c r="I64" t="n">
-        <v>0.8693310996769175</v>
+        <v>0.8829256708620281</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Cromossoma 8</t>
+          <t>Cromossoma 9</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>1380.539651173995</v>
+        <v>1462.841550770668</v>
       </c>
       <c r="D65" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E65" t="n">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="F65" t="n">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="G65" t="n">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="H65" t="n">
-        <v>0.009094172549958118</v>
+        <v>0.009617668012348611</v>
       </c>
       <c r="I65" t="n">
-        <v>0.8784252722268756</v>
+        <v>0.8925433388743768</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Cromossoma 24</t>
+          <t>Cromossoma 79</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1483.717763167424</v>
+        <v>1481.253662385921</v>
       </c>
       <c r="D66" t="n">
         <v>15</v>
       </c>
       <c r="E66" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F66" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G66" t="n">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H66" t="n">
-        <v>0.008974512384827091</v>
+        <v>0.008430301591071004</v>
       </c>
       <c r="I66" t="n">
-        <v>0.8873997846117027</v>
+        <v>0.9009736404654478</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Cromossoma 20</t>
+          <t>Cromossoma 13</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1489.282825052043</v>
+        <v>1486.75018077292</v>
       </c>
       <c r="D67" t="n">
         <v>15</v>
       </c>
       <c r="E67" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F67" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G67" t="n">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H67" t="n">
-        <v>0.008735192054565036</v>
+        <v>0.008192828306815484</v>
       </c>
       <c r="I67" t="n">
-        <v>0.8961349766662677</v>
+        <v>0.9091664687722633</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Cromossoma 76</t>
+          <t>Cromossoma 33</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1493.548082311969</v>
+        <v>1487.420824023489</v>
       </c>
       <c r="D68" t="n">
         <v>15</v>
       </c>
       <c r="E68" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F68" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G68" t="n">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H68" t="n">
-        <v>0.008615531889434008</v>
+        <v>0.008074091664687722</v>
       </c>
       <c r="I68" t="n">
-        <v>0.9047505085557017</v>
+        <v>0.917240560436951</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Cromossoma 16</t>
+          <t>Cromossoma 1</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1504.473753644467</v>
+        <v>1499.813623370351</v>
       </c>
       <c r="D69" t="n">
         <v>15</v>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F69" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G69" t="n">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H69" t="n">
-        <v>0.008256551394040924</v>
+        <v>0.00771788173830444</v>
       </c>
       <c r="I69" t="n">
-        <v>0.9130070599497426</v>
+        <v>0.9249584421752555</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Cromossoma 73</t>
+          <t>Cromossoma 53</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1516.292438305556</v>
+        <v>1501.875318529548</v>
       </c>
       <c r="D70" t="n">
         <v>15</v>
       </c>
       <c r="E70" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F70" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G70" t="n">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H70" t="n">
-        <v>0.008136891228909897</v>
+        <v>0.00759914509617668</v>
       </c>
       <c r="I70" t="n">
-        <v>0.9211439511786526</v>
+        <v>0.9325575872714321</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Cromossoma 26</t>
+          <t>Cromossoma 16</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>1404.24805364682</v>
+        <v>1511.959532512278</v>
       </c>
       <c r="D71" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E71" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F71" t="n">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="G71" t="n">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="H71" t="n">
-        <v>0.008136891228909897</v>
+        <v>0.007480408454048919</v>
       </c>
       <c r="I71" t="n">
-        <v>0.9292808424075625</v>
+        <v>0.9400379957254811</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Cromossoma 60</t>
+          <t>Cromossoma 83</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>1543.874358685827</v>
+        <v>1513.91903576358</v>
       </c>
       <c r="D72" t="n">
         <v>15</v>
       </c>
       <c r="E72" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F72" t="n">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G72" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H72" t="n">
-        <v>0.007658250568385785</v>
+        <v>0.007361671811921159</v>
       </c>
       <c r="I72" t="n">
-        <v>0.9369390929759482</v>
+        <v>0.9473996675374022</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Cromossoma 62</t>
+          <t>Cromossoma 82</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>1412.932568948913</v>
+        <v>1519.628830601122</v>
       </c>
       <c r="D73" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E73" t="n">
-        <v>46</v>
+        <v>6</v>
       </c>
       <c r="F73" t="n">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="G73" t="n">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="H73" t="n">
-        <v>0.007658250568385785</v>
+        <v>0.007005461885537877</v>
       </c>
       <c r="I73" t="n">
-        <v>0.944597343544334</v>
+        <v>0.9544051294229401</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>57</v>
+        <v>5</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Cromossoma 57</t>
+          <t>Cromossoma 5</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>1372.882458931758</v>
+        <v>1543.417993500461</v>
       </c>
       <c r="D74" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E74" t="n">
-        <v>62</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="G74" t="n">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H74" t="n">
-        <v>0.007658250568385785</v>
+        <v>0.006886725243410117</v>
       </c>
       <c r="I74" t="n">
-        <v>0.9522555941127198</v>
+        <v>0.9612918546663503</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Cromossoma 79</t>
+          <t>Cromossoma 40</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>1618.332755542851</v>
+        <v>1405.349998398815</v>
       </c>
       <c r="D75" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E75" t="n">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="F75" t="n">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="G75" t="n">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H75" t="n">
-        <v>0.007418930238123729</v>
+        <v>0.006767988601282355</v>
       </c>
       <c r="I75" t="n">
-        <v>0.9596745243508434</v>
+        <v>0.9680598432676326</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Cromossoma 29</t>
+          <t>Cromossoma 52</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>1429.210475710702</v>
+        <v>1411.316124067568</v>
       </c>
       <c r="D76" t="n">
         <v>16</v>
       </c>
       <c r="E76" t="n">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="F76" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G76" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H76" t="n">
-        <v>0.006700969247337561</v>
+        <v>0.006530515317026834</v>
       </c>
       <c r="I76" t="n">
-        <v>0.966375493598181</v>
+        <v>0.9745903585846595</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Cromossoma 41</t>
+          <t>Cromossoma 14</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>1442.223862967191</v>
+        <v>1459.512158474143</v>
       </c>
       <c r="D77" t="n">
         <v>16</v>
       </c>
       <c r="E77" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F77" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G77" t="n">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H77" t="n">
-        <v>0.005863348091420366</v>
+        <v>0.004868202327238186</v>
       </c>
       <c r="I77" t="n">
-        <v>0.9722388416896014</v>
+        <v>0.9794585609118976</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Cromossoma 11</t>
+          <t>Cromossoma 49</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>1449.915327833377</v>
+        <v>1465.812864461991</v>
       </c>
       <c r="D78" t="n">
         <v>16</v>
       </c>
       <c r="E78" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F78" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G78" t="n">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H78" t="n">
-        <v>0.005145387100634199</v>
+        <v>0.004274519116599383</v>
       </c>
       <c r="I78" t="n">
-        <v>0.9773842287902356</v>
+        <v>0.983733080028497</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Cromossoma 55</t>
+          <t>Cromossoma 28</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>1453.791004604195</v>
+        <v>1485.660711725866</v>
       </c>
       <c r="D79" t="n">
         <v>16</v>
       </c>
       <c r="E79" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="F79" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G79" t="n">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="H79" t="n">
-        <v>0.004906066770372143</v>
+        <v>0.003443362621705058</v>
       </c>
       <c r="I79" t="n">
-        <v>0.9822902955606078</v>
+        <v>0.9871764426502021</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Cromossoma 27</t>
+          <t>Cromossoma 65</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>1469.401553945375</v>
+        <v>1494.403992414278</v>
       </c>
       <c r="D80" t="n">
         <v>16</v>
       </c>
       <c r="E80" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F80" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G80" t="n">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="H80" t="n">
-        <v>0.004307765944717004</v>
+        <v>0.003087152695321776</v>
       </c>
       <c r="I80" t="n">
-        <v>0.9865980615053248</v>
+        <v>0.9902635953455239</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Cromossoma 49</t>
+          <t>Cromossoma 10</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>1486.764902971244</v>
+        <v>1495.028591164936</v>
       </c>
       <c r="D81" t="n">
         <v>16</v>
@@ -2943,137 +2943,137 @@
         <v>13</v>
       </c>
       <c r="F81" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G81" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H81" t="n">
-        <v>0.003709465119061864</v>
+        <v>0.002968416053194016</v>
       </c>
       <c r="I81" t="n">
-        <v>0.9903075266243867</v>
+        <v>0.9932320113987179</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Cromossoma 23</t>
+          <t>Cromossoma 7</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>1525.391812226194</v>
+        <v>1514.016675544369</v>
       </c>
       <c r="D82" t="n">
         <v>16</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F82" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G82" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H82" t="n">
-        <v>0.002871843963144669</v>
+        <v>0.002374732842555213</v>
       </c>
       <c r="I82" t="n">
-        <v>0.9931793705875314</v>
+        <v>0.995606744241273</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>83</v>
+        <v>36</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Cromossoma 83</t>
+          <t>Cromossoma 36</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>1533.027080657619</v>
+        <v>1516.590031495921</v>
       </c>
       <c r="D83" t="n">
         <v>16</v>
       </c>
       <c r="E83" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F83" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G83" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H83" t="n">
-        <v>0.002752183798013641</v>
+        <v>0.002255996200427452</v>
       </c>
       <c r="I83" t="n">
-        <v>0.995931554385545</v>
+        <v>0.9978627404417005</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Cromossoma 78</t>
+          <t>Cromossoma 37</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>1541.397813038245</v>
+        <v>1565.724874556885</v>
       </c>
       <c r="D84" t="n">
         <v>16</v>
       </c>
       <c r="E84" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G84" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H84" t="n">
-        <v>0.002632523632882613</v>
+        <v>0.001662312989788649</v>
       </c>
       <c r="I84" t="n">
-        <v>0.9985640780184276</v>
+        <v>0.9995250534314892</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Cromossoma 74</t>
+          <t>Cromossoma 60</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>1495.613904028962</v>
+        <v>1563.754639728299</v>
       </c>
       <c r="D85" t="n">
         <v>17</v>
       </c>
       <c r="E85" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G85" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H85" t="n">
-        <v>0.001435921981572335</v>
+        <v>0.0004749465685110425</v>
       </c>
       <c r="I85" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
20220310 Confirmação Mutação e Cruzamento AEX
</commit_message>
<xml_diff>
--- a/Dados/Debug/Roleta_Debug.xlsx
+++ b/Dados/Debug/Roleta_Debug.xlsx
@@ -477,263 +477,263 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cromossoma 51</t>
+          <t>Cromossoma 24</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1293.915830202608</v>
+        <v>1258.155462688554</v>
       </c>
       <c r="D2" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" t="n">
         <v>83</v>
       </c>
       <c r="F2" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G2" t="n">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H2" t="n">
-        <v>0.02025961421812447</v>
+        <v>0.01943566327127971</v>
       </c>
       <c r="I2" t="n">
-        <v>0.02025961421812447</v>
+        <v>0.01943566327127971</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cromossoma 28</t>
+          <t>Cromossoma 53</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1302.878906987785</v>
+        <v>1263.164564607314</v>
       </c>
       <c r="D3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F3" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G3" t="n">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H3" t="n">
-        <v>0.01989566905252942</v>
+        <v>0.01931858096241658</v>
       </c>
       <c r="I3" t="n">
-        <v>0.04015528327065389</v>
+        <v>0.03875424423369629</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Cromossoma 17</t>
+          <t>Cromossoma 13</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1295.193702058407</v>
+        <v>1307.413874005071</v>
       </c>
       <c r="D4" t="n">
         <v>14</v>
       </c>
       <c r="E4" t="n">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F4" t="n">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G4" t="n">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="H4" t="n">
-        <v>0.01941040883173602</v>
+        <v>0.01908441634469032</v>
       </c>
       <c r="I4" t="n">
-        <v>0.05956569210238991</v>
+        <v>0.05783866057838661</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Cromossoma 34</t>
+          <t>Cromossoma 72</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1317.353021631123</v>
+        <v>1330.168363200362</v>
       </c>
       <c r="D5" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" t="n">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F5" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G5" t="n">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H5" t="n">
-        <v>0.01928909377653767</v>
+        <v>0.01885025172696406</v>
       </c>
       <c r="I5" t="n">
-        <v>0.07885478587892758</v>
+        <v>0.07668891230535066</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Cromossoma 3</t>
+          <t>Cromossoma 22</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1304.43574589977</v>
+        <v>1344.523447276128</v>
       </c>
       <c r="D6" t="n">
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F6" t="n">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G6" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H6" t="n">
-        <v>0.01904646366614097</v>
+        <v>0.01849900480037466</v>
       </c>
       <c r="I6" t="n">
-        <v>0.09790124954506854</v>
+        <v>0.09518791710572533</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cromossoma 40</t>
+          <t>Cromossoma 57</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1335.21902339968</v>
+        <v>1346.924943076636</v>
       </c>
       <c r="D7" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F7" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G7" t="n">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H7" t="n">
-        <v>0.01880383355574427</v>
+        <v>0.01838192249151153</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1167050831008128</v>
+        <v>0.1135698395972369</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Cromossoma 83</t>
+          <t>Cromossoma 82</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1320.01606387169</v>
+        <v>1354.430168242386</v>
       </c>
       <c r="D8" t="n">
         <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F8" t="n">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G8" t="n">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H8" t="n">
-        <v>0.01843988839014922</v>
+        <v>0.01814775787378527</v>
       </c>
       <c r="I8" t="n">
-        <v>0.135144971490962</v>
+        <v>0.1317175974710221</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>80</v>
+        <v>23</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Cromossoma 80</t>
+          <t>Cromossoma 23</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1322.828226277374</v>
+        <v>1362.450290218126</v>
       </c>
       <c r="D9" t="n">
         <v>14</v>
       </c>
       <c r="E9" t="n">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F9" t="n">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G9" t="n">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H9" t="n">
-        <v>0.01831857333495087</v>
+        <v>0.01803067556492214</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1534635448259129</v>
+        <v>0.1497482730359443</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Cromossoma 67</t>
+          <t>Cromossoma 56</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1339.260642491366</v>
+        <v>1367.452258903949</v>
       </c>
       <c r="D10" t="n">
         <v>14</v>
@@ -742,494 +742,494 @@
         <v>70</v>
       </c>
       <c r="F10" t="n">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G10" t="n">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="H10" t="n">
-        <v>0.01795462816935582</v>
+        <v>0.01791359325605901</v>
       </c>
       <c r="I10" t="n">
-        <v>0.1714181729952687</v>
+        <v>0.1676618662920033</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Cromossoma 73</t>
+          <t>Cromossoma 76</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1340.884670285615</v>
+        <v>1371.464250490414</v>
       </c>
       <c r="D11" t="n">
         <v>14</v>
       </c>
       <c r="E11" t="n">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F11" t="n">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G11" t="n">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="H11" t="n">
-        <v>0.01783331311415747</v>
+        <v>0.01767942863833275</v>
       </c>
       <c r="I11" t="n">
-        <v>0.1892514861094262</v>
+        <v>0.185341294930336</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Cromossoma 7</t>
+          <t>Cromossoma 40</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>1345.607066104839</v>
+        <v>1373.644256429958</v>
       </c>
       <c r="D12" t="n">
         <v>14</v>
       </c>
       <c r="E12" t="n">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F12" t="n">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G12" t="n">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="H12" t="n">
-        <v>0.01771199805895912</v>
+        <v>0.01744526402060649</v>
       </c>
       <c r="I12" t="n">
-        <v>0.2069634841683853</v>
+        <v>0.2027865589509425</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Cromossoma 71</t>
+          <t>Cromossoma 51</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>1297.87129896012</v>
+        <v>1378.550347287579</v>
       </c>
       <c r="D13" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" t="n">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="F13" t="n">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="G13" t="n">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="H13" t="n">
-        <v>0.01698410772776902</v>
+        <v>0.01721109940288023</v>
       </c>
       <c r="I13" t="n">
-        <v>0.2239475918961543</v>
+        <v>0.2199976583538227</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Cromossoma 32</t>
+          <t>Cromossoma 58</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1391.653529956294</v>
+        <v>1381.931015399535</v>
       </c>
       <c r="D14" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E14" t="n">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F14" t="n">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G14" t="n">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="H14" t="n">
-        <v>0.01662016256217396</v>
+        <v>0.01685985247629083</v>
       </c>
       <c r="I14" t="n">
-        <v>0.2405677544583283</v>
+        <v>0.2368575108301136</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Cromossoma 0</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1382.172990947954</v>
+      </c>
+      <c r="D15" t="n">
         <v>14</v>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Cromossoma 14</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>1312.016945421185</v>
-      </c>
-      <c r="D15" t="n">
-        <v>15</v>
-      </c>
       <c r="E15" t="n">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="F15" t="n">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="G15" t="n">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="H15" t="n">
-        <v>0.01662016256217396</v>
+        <v>0.0167427701674277</v>
       </c>
       <c r="I15" t="n">
-        <v>0.2571879170205023</v>
+        <v>0.2536002809975413</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Cromossoma 16</t>
+          <t>Cromossoma 71</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1324.287475436964</v>
+        <v>1220.797969397157</v>
       </c>
       <c r="D16" t="n">
         <v>15</v>
       </c>
       <c r="E16" t="n">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="F16" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G16" t="n">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="H16" t="n">
-        <v>0.01589227223098387</v>
+        <v>0.01662568785856457</v>
       </c>
       <c r="I16" t="n">
-        <v>0.2730801892514861</v>
+        <v>0.2702259688561058</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Cromossoma 50</t>
+          <t>Cromossoma 63</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1391.66468510753</v>
+        <v>1313.465141892968</v>
       </c>
       <c r="D17" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E17" t="n">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="F17" t="n">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="G17" t="n">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="H17" t="n">
-        <v>0.01577095717578551</v>
+        <v>0.01604027631424892</v>
       </c>
       <c r="I17" t="n">
-        <v>0.2888511464272717</v>
+        <v>0.2862662451703548</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Cromossoma 74</t>
+          <t>Cromossoma 59</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1392.844557640051</v>
+        <v>1338.042257335269</v>
       </c>
       <c r="D18" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E18" t="n">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="F18" t="n">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="G18" t="n">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="H18" t="n">
-        <v>0.01564964212058716</v>
+        <v>0.01580611169652266</v>
       </c>
       <c r="I18" t="n">
-        <v>0.3045007885478588</v>
+        <v>0.3020723568668774</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>81</v>
+        <v>28</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Cromossoma 81</t>
+          <t>Cromossoma 28</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1402.992058187763</v>
+        <v>1343.663377110486</v>
       </c>
       <c r="D19" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E19" t="n">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="F19" t="n">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="G19" t="n">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="H19" t="n">
-        <v>0.01528569695499211</v>
+        <v>0.01568902938765953</v>
       </c>
       <c r="I19" t="n">
-        <v>0.3197864855028509</v>
+        <v>0.3177613862545369</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Cromossoma 24</t>
+          <t>Cromossoma 60</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1346.757468668663</v>
+        <v>1409.717034799425</v>
       </c>
       <c r="D20" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" t="n">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="F20" t="n">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="G20" t="n">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H20" t="n">
-        <v>0.01528569695499211</v>
+        <v>0.01510361784334387</v>
       </c>
       <c r="I20" t="n">
-        <v>0.335072182457843</v>
+        <v>0.3328650040978808</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Cromossoma 37</t>
+          <t>Cromossoma 79</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1351.068346123225</v>
+        <v>1411.392727747084</v>
       </c>
       <c r="D21" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E21" t="n">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="F21" t="n">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="G21" t="n">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H21" t="n">
-        <v>0.01516438189979376</v>
+        <v>0.01486945322561761</v>
       </c>
       <c r="I21" t="n">
-        <v>0.3502365643576368</v>
+        <v>0.3477344573234984</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>4</v>
+        <v>74</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Cromossoma 4</t>
+          <t>Cromossoma 74</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1408.032288444696</v>
+        <v>1369.494088230404</v>
       </c>
       <c r="D22" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E22" t="n">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="F22" t="n">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="G22" t="n">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="H22" t="n">
-        <v>0.01504306684459541</v>
+        <v>0.01486945322561761</v>
       </c>
       <c r="I22" t="n">
-        <v>0.3652796312022322</v>
+        <v>0.362603910549116</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Cromossoma 76</t>
+          <t>Cromossoma 9</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1353.221881066873</v>
+        <v>1372.128282460611</v>
       </c>
       <c r="D23" t="n">
         <v>15</v>
       </c>
       <c r="E23" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F23" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G23" t="n">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H23" t="n">
-        <v>0.01504306684459541</v>
+        <v>0.01463528860789135</v>
       </c>
       <c r="I23" t="n">
-        <v>0.3803226980468276</v>
+        <v>0.3772391991570074</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Cromossoma 55</t>
+          <t>Cromossoma 35</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1360.603474852481</v>
+        <v>1374.685505863701</v>
       </c>
       <c r="D24" t="n">
         <v>15</v>
       </c>
       <c r="E24" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F24" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G24" t="n">
         <v>123</v>
       </c>
       <c r="H24" t="n">
-        <v>0.01492175178939706</v>
+        <v>0.01440112399016509</v>
       </c>
       <c r="I24" t="n">
-        <v>0.3952444498362246</v>
+        <v>0.3916403231471725</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Cromossoma 12</t>
+          <t>Cromossoma 64</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1361.746815514281</v>
+        <v>1428.246702605157</v>
       </c>
       <c r="D25" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E25" t="n">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="F25" t="n">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="G25" t="n">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H25" t="n">
-        <v>0.01480043673419871</v>
+        <v>0.01404987706357569</v>
       </c>
       <c r="I25" t="n">
-        <v>0.4100448865704234</v>
+        <v>0.4056902002107481</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Cromossoma 9</t>
+          <t>Cromossoma 61</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1368.468602525638</v>
+        <v>1380.108853356158</v>
       </c>
       <c r="D26" t="n">
         <v>15</v>
@@ -1238,1842 +1238,1842 @@
         <v>62</v>
       </c>
       <c r="F26" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G26" t="n">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H26" t="n">
-        <v>0.01467912167900036</v>
+        <v>0.01404987706357569</v>
       </c>
       <c r="I26" t="n">
-        <v>0.4247240082494237</v>
+        <v>0.4197400772743238</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Cromossoma 19</t>
+          <t>Cromossoma 78</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1378.528882981956</v>
+        <v>1429.932469014709</v>
       </c>
       <c r="D27" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E27" t="n">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="F27" t="n">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="G27" t="n">
         <v>119</v>
       </c>
       <c r="H27" t="n">
-        <v>0.01443649156860366</v>
+        <v>0.01393279475471256</v>
       </c>
       <c r="I27" t="n">
-        <v>0.4391604998180274</v>
+        <v>0.4336728720290364</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Cromossoma 8</t>
+          <t>Cromossoma 36</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1420.484527832818</v>
+        <v>1384.668357435472</v>
       </c>
       <c r="D28" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E28" t="n">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="F28" t="n">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="G28" t="n">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H28" t="n">
-        <v>0.01443649156860366</v>
+        <v>0.0136986301369863</v>
       </c>
       <c r="I28" t="n">
-        <v>0.4535969913866311</v>
+        <v>0.4473715021660227</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>82</v>
+        <v>29</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Cromossoma 82</t>
+          <t>Cromossoma 29</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>1422.626772707571</v>
+        <v>1385.699726011023</v>
       </c>
       <c r="D29" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E29" t="n">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="F29" t="n">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="G29" t="n">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H29" t="n">
-        <v>0.01431517651340531</v>
+        <v>0.01358154782812317</v>
       </c>
       <c r="I29" t="n">
-        <v>0.4679121679000364</v>
+        <v>0.4609530499941458</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Cromossoma 1</t>
+          <t>Cromossoma 70</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1383.284194713204</v>
+        <v>1388.209088885934</v>
       </c>
       <c r="D30" t="n">
         <v>15</v>
       </c>
       <c r="E30" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F30" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G30" t="n">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H30" t="n">
-        <v>0.01431517651340531</v>
+        <v>0.01346446551926004</v>
       </c>
       <c r="I30" t="n">
-        <v>0.4822273444134417</v>
+        <v>0.4744175155134059</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Cromossoma 72</t>
+          <t>Cromossoma 18</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>1384.331984107701</v>
+        <v>1390.011352515372</v>
       </c>
       <c r="D31" t="n">
         <v>15</v>
       </c>
       <c r="E31" t="n">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F31" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G31" t="n">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H31" t="n">
-        <v>0.01419386145820696</v>
+        <v>0.01334738321039691</v>
       </c>
       <c r="I31" t="n">
-        <v>0.4964212058716486</v>
+        <v>0.4877648987238028</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Cromossoma 45</t>
+          <t>Cromossoma 41</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1430.960646484843</v>
+        <v>1390.970913865467</v>
       </c>
       <c r="D32" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E32" t="n">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="F32" t="n">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="G32" t="n">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H32" t="n">
-        <v>0.01407254640300861</v>
+        <v>0.01323030090153378</v>
       </c>
       <c r="I32" t="n">
-        <v>0.5104937522746572</v>
+        <v>0.5009951996253366</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Cromossoma 48</t>
+          <t>Cromossoma 42</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1384.859014575579</v>
+        <v>1397.822130630478</v>
       </c>
       <c r="D33" t="n">
         <v>15</v>
       </c>
       <c r="E33" t="n">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F33" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G33" t="n">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H33" t="n">
-        <v>0.01407254640300861</v>
+        <v>0.01311321859267065</v>
       </c>
       <c r="I33" t="n">
-        <v>0.5245662986776658</v>
+        <v>0.5141084182180072</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Cromossoma 47</t>
+          <t>Cromossoma 44</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1385.1499386478</v>
+        <v>1399.69908564188</v>
       </c>
       <c r="D34" t="n">
         <v>15</v>
       </c>
       <c r="E34" t="n">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F34" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G34" t="n">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H34" t="n">
-        <v>0.01395123134781026</v>
+        <v>0.01299613628380752</v>
       </c>
       <c r="I34" t="n">
-        <v>0.5385175300254761</v>
+        <v>0.5271045545018147</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Cromossoma 27</t>
+          <t>Cromossoma 11</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1391.254625900591</v>
+        <v>1401.026717147551</v>
       </c>
       <c r="D35" t="n">
         <v>15</v>
       </c>
       <c r="E35" t="n">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F35" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G35" t="n">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H35" t="n">
-        <v>0.01370860123741356</v>
+        <v>0.01287905397494439</v>
       </c>
       <c r="I35" t="n">
-        <v>0.5522261312628897</v>
+        <v>0.5399836084767591</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Cromossoma 61</t>
+          <t>Cromossoma 20</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>1402.428892702821</v>
+        <v>1451.610472449456</v>
       </c>
       <c r="D36" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E36" t="n">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="F36" t="n">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="G36" t="n">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H36" t="n">
-        <v>0.01310202596142181</v>
+        <v>0.01287905397494439</v>
       </c>
       <c r="I36" t="n">
-        <v>0.5653281572243115</v>
+        <v>0.5528626624517035</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Cromossoma 75</t>
+          <t>Cromossoma 33</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>1462.386085595315</v>
+        <v>1402.29092511053</v>
       </c>
       <c r="D37" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E37" t="n">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="F37" t="n">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="G37" t="n">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H37" t="n">
-        <v>0.01310202596142181</v>
+        <v>0.01276197166608125</v>
       </c>
       <c r="I37" t="n">
-        <v>0.5784301831857334</v>
+        <v>0.5656246341177847</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Cromossoma 2</t>
+          <t>Cromossoma 46</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1452.512826568618</v>
+        <v>1451.976195572162</v>
       </c>
       <c r="D38" t="n">
         <v>14</v>
       </c>
       <c r="E38" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F38" t="n">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G38" t="n">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H38" t="n">
-        <v>0.01310202596142181</v>
+        <v>0.01276197166608125</v>
       </c>
       <c r="I38" t="n">
-        <v>0.5915322091471552</v>
+        <v>0.578386605783866</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Cromossoma 46</t>
+          <t>Cromossoma 55</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1406.755487593515</v>
+        <v>1405.501169108064</v>
       </c>
       <c r="D39" t="n">
         <v>15</v>
       </c>
       <c r="E39" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F39" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G39" t="n">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H39" t="n">
-        <v>0.01285939585102511</v>
+        <v>0.01264488935721812</v>
       </c>
       <c r="I39" t="n">
-        <v>0.6043916049981803</v>
+        <v>0.5910314951410841</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Cromossoma 57</t>
+          <t>Cromossoma 8</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1408.652749938713</v>
+        <v>1406.595730343208</v>
       </c>
       <c r="D40" t="n">
         <v>15</v>
       </c>
       <c r="E40" t="n">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F40" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G40" t="n">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H40" t="n">
-        <v>0.01261676574062841</v>
+        <v>0.01252780704835499</v>
       </c>
       <c r="I40" t="n">
-        <v>0.6170083707388088</v>
+        <v>0.6035593021894391</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Cromossoma 21</t>
+          <t>Cromossoma 49</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1281.690569498116</v>
+        <v>1406.787382723093</v>
       </c>
       <c r="D41" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E41" t="n">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="F41" t="n">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="G41" t="n">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H41" t="n">
-        <v>0.01249545068543006</v>
+        <v>0.01241072473949186</v>
       </c>
       <c r="I41" t="n">
-        <v>0.6295038214242388</v>
+        <v>0.615970026928931</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Cromossoma 11</t>
+          <t>Cromossoma 6</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1414.789138269999</v>
+        <v>1408.172546050421</v>
       </c>
       <c r="D42" t="n">
         <v>15</v>
       </c>
       <c r="E42" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F42" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G42" t="n">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H42" t="n">
-        <v>0.01249545068543006</v>
+        <v>0.01229364243062873</v>
       </c>
       <c r="I42" t="n">
-        <v>0.6419992721096688</v>
+        <v>0.6282636693595597</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Cromossoma 31</t>
+          <t>Cromossoma 77</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1418.472167492175</v>
+        <v>1469.633976306856</v>
       </c>
       <c r="D43" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E43" t="n">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F43" t="n">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="G43" t="n">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H43" t="n">
-        <v>0.01237413563023171</v>
+        <v>0.0121765601217656</v>
       </c>
       <c r="I43" t="n">
-        <v>0.6543734077399005</v>
+        <v>0.6404402294813253</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>58</v>
+        <v>2</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Cromossoma 58</t>
+          <t>Cromossoma 2</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1420.182762966239</v>
+        <v>1475.217484817921</v>
       </c>
       <c r="D44" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E44" t="n">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="F44" t="n">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="G44" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H44" t="n">
-        <v>0.01225282057503336</v>
+        <v>0.01205947781290247</v>
       </c>
       <c r="I44" t="n">
-        <v>0.6666262283149339</v>
+        <v>0.6524997072942278</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Cromossoma 66</t>
+          <t>Cromossoma 65</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1464.522404932418</v>
+        <v>1410.030757386952</v>
       </c>
       <c r="D45" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E45" t="n">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="F45" t="n">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="G45" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H45" t="n">
-        <v>0.01225282057503336</v>
+        <v>0.01205947781290247</v>
       </c>
       <c r="I45" t="n">
-        <v>0.6788790488899673</v>
+        <v>0.6645591851071303</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>20</v>
+        <v>83</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Cromossoma 20</t>
+          <t>Cromossoma 83</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1313.513601002429</v>
+        <v>1410.088754026931</v>
       </c>
       <c r="D46" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E46" t="n">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="F46" t="n">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="G46" t="n">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="H46" t="n">
-        <v>0.01164624529904161</v>
+        <v>0.01194239550403934</v>
       </c>
       <c r="I46" t="n">
-        <v>0.6905252941890089</v>
+        <v>0.6765015806111696</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Cromossoma 0</t>
+          <t>Cromossoma 25</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>1435.150248412144</v>
+        <v>1414.212193883911</v>
       </c>
       <c r="D47" t="n">
         <v>15</v>
       </c>
       <c r="E47" t="n">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="F47" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G47" t="n">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="H47" t="n">
-        <v>0.01164624529904161</v>
+        <v>0.01170823088631308</v>
       </c>
       <c r="I47" t="n">
-        <v>0.7021715394880504</v>
+        <v>0.6882098114974827</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Cromossoma 39</t>
+          <t>Cromossoma 43</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1314.885849076852</v>
+        <v>1424.760422311531</v>
       </c>
       <c r="D48" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E48" t="n">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="F48" t="n">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="G48" t="n">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H48" t="n">
-        <v>0.01152493024384326</v>
+        <v>0.01147406626858682</v>
       </c>
       <c r="I48" t="n">
-        <v>0.7136964697318937</v>
+        <v>0.6996838777660696</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Cromossoma 30</t>
+          <t>Cromossoma 15</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1476.389820273438</v>
+        <v>1484.259807153725</v>
       </c>
       <c r="D49" t="n">
         <v>14</v>
       </c>
       <c r="E49" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F49" t="n">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="G49" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H49" t="n">
-        <v>0.01152493024384326</v>
+        <v>0.01135698395972369</v>
       </c>
       <c r="I49" t="n">
-        <v>0.725221399975737</v>
+        <v>0.7110408617257933</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Cromossoma 10</t>
+          <t>Cromossoma 16</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1441.900941912201</v>
+        <v>1425.404260637257</v>
       </c>
       <c r="D50" t="n">
         <v>15</v>
       </c>
       <c r="E50" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F50" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G50" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H50" t="n">
-        <v>0.01152493024384326</v>
+        <v>0.01135698395972369</v>
       </c>
       <c r="I50" t="n">
-        <v>0.7367463302195802</v>
+        <v>0.722397845685517</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Cromossoma 42</t>
+          <t>Cromossoma 14</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1443.352675550698</v>
+        <v>1428.180999308006</v>
       </c>
       <c r="D51" t="n">
         <v>15</v>
       </c>
       <c r="E51" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F51" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G51" t="n">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H51" t="n">
-        <v>0.01140361518864491</v>
+        <v>0.01123990165086055</v>
       </c>
       <c r="I51" t="n">
-        <v>0.7481499454082252</v>
+        <v>0.7336377473363775</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Cromossoma 69</t>
+          <t>Cromossoma 3</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1447.647248775437</v>
+        <v>1488.503263784041</v>
       </c>
       <c r="D52" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E52" t="n">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="F52" t="n">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="G52" t="n">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H52" t="n">
-        <v>0.01128230013344656</v>
+        <v>0.01112281934199742</v>
       </c>
       <c r="I52" t="n">
-        <v>0.7594322455416718</v>
+        <v>0.744760566678375</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Cromossoma 35</t>
+          <t>Cromossoma 54</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1483.680421817922</v>
+        <v>1270.79645268163</v>
       </c>
       <c r="D53" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E53" t="n">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="F53" t="n">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="G53" t="n">
         <v>93</v>
       </c>
       <c r="H53" t="n">
-        <v>0.01128230013344656</v>
+        <v>0.01088865472427116</v>
       </c>
       <c r="I53" t="n">
-        <v>0.7707145456751183</v>
+        <v>0.7556492214026461</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Cromossoma 6</t>
+          <t>Cromossoma 5</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1452.076396700039</v>
+        <v>1436.454405949466</v>
       </c>
       <c r="D54" t="n">
         <v>15</v>
       </c>
       <c r="E54" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F54" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G54" t="n">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H54" t="n">
-        <v>0.01091835496785151</v>
+        <v>0.01088865472427116</v>
       </c>
       <c r="I54" t="n">
-        <v>0.7816329006429699</v>
+        <v>0.7665378761269173</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Cromossoma 52</t>
+          <t>Cromossoma 21</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1459.870938525195</v>
+        <v>1437.615342962999</v>
       </c>
       <c r="D55" t="n">
         <v>15</v>
       </c>
       <c r="E55" t="n">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F55" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G55" t="n">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="H55" t="n">
-        <v>0.01043309474705811</v>
+        <v>0.01077157241540803</v>
       </c>
       <c r="I55" t="n">
-        <v>0.792065995390028</v>
+        <v>0.7773094485423253</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Cromossoma 56</t>
+          <t>Cromossoma 39</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>1461.496864379824</v>
+        <v>1438.899952071488</v>
       </c>
       <c r="D56" t="n">
         <v>15</v>
       </c>
       <c r="E56" t="n">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F56" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G56" t="n">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="H56" t="n">
-        <v>0.01031177969185976</v>
+        <v>0.0106544901065449</v>
       </c>
       <c r="I56" t="n">
-        <v>0.8023777750818878</v>
+        <v>0.7879639386488702</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Cromossoma 53</t>
+          <t>Cromossoma 50</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>1461.501680373299</v>
+        <v>1512.791900001893</v>
       </c>
       <c r="D57" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E57" t="n">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="F57" t="n">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="G57" t="n">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="H57" t="n">
-        <v>0.01019046463666141</v>
+        <v>0.01053740779768177</v>
       </c>
       <c r="I57" t="n">
-        <v>0.8125682397185492</v>
+        <v>0.7985013464465519</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Cromossoma 22</t>
+          <t>Cromossoma 38</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1541.473975951142</v>
+        <v>1442.015640197786</v>
       </c>
       <c r="D58" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E58" t="n">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="F58" t="n">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="G58" t="n">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="H58" t="n">
-        <v>0.01019046463666141</v>
+        <v>0.01053740779768177</v>
       </c>
       <c r="I58" t="n">
-        <v>0.8227587043552106</v>
+        <v>0.8090387542442337</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Cromossoma 13</t>
+          <t>Cromossoma 62</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>1464.89841014299</v>
+        <v>1513.91418448466</v>
       </c>
       <c r="D59" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E59" t="n">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="F59" t="n">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="G59" t="n">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="H59" t="n">
-        <v>0.00982651947106636</v>
+        <v>0.01042032548881864</v>
       </c>
       <c r="I59" t="n">
-        <v>0.832585223826277</v>
+        <v>0.8194590797330523</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Cromossoma 25</t>
+          <t>Cromossoma 27</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1377.452644230926</v>
+        <v>1445.457348595379</v>
       </c>
       <c r="D60" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E60" t="n">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="F60" t="n">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="G60" t="n">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="H60" t="n">
-        <v>0.009705204415868009</v>
+        <v>0.01042032548881864</v>
       </c>
       <c r="I60" t="n">
-        <v>0.842290428242145</v>
+        <v>0.829879405221871</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Cromossoma 5</t>
+          <t>Cromossoma 47</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>1474.51034825098</v>
+        <v>1447.578635610252</v>
       </c>
       <c r="D61" t="n">
         <v>15</v>
       </c>
       <c r="E61" t="n">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F61" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G61" t="n">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="H61" t="n">
-        <v>0.009462574305471309</v>
+        <v>0.01030324317995551</v>
       </c>
       <c r="I61" t="n">
-        <v>0.8517530025476162</v>
+        <v>0.8401826484018264</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Cromossoma 41</t>
+          <t>Cromossoma 34</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1475.103407039656</v>
+        <v>1449.060109721396</v>
       </c>
       <c r="D62" t="n">
         <v>15</v>
       </c>
       <c r="E62" t="n">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F62" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G62" t="n">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="H62" t="n">
-        <v>0.00934125925027296</v>
+        <v>0.01018616087109238</v>
       </c>
       <c r="I62" t="n">
-        <v>0.8610942617978892</v>
+        <v>0.8503688092729188</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Cromossoma 29</t>
+          <t>Cromossoma 67</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1482.989653134426</v>
+        <v>1449.509449272464</v>
       </c>
       <c r="D63" t="n">
         <v>15</v>
       </c>
       <c r="E63" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F63" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G63" t="n">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="H63" t="n">
-        <v>0.009098629139876259</v>
+        <v>0.01006907856222925</v>
       </c>
       <c r="I63" t="n">
-        <v>0.8701928909377654</v>
+        <v>0.8604378878351481</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Cromossoma 64</t>
+          <t>Cromossoma 52</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1386.078923510748</v>
+        <v>1350.678935605421</v>
       </c>
       <c r="D64" t="n">
         <v>16</v>
       </c>
       <c r="E64" t="n">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="F64" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G64" t="n">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="H64" t="n">
-        <v>0.008977314084677909</v>
+        <v>0.009951996253366116</v>
       </c>
       <c r="I64" t="n">
-        <v>0.8791702050224434</v>
+        <v>0.8703898840885141</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Cromossoma 60</t>
+          <t>Cromossoma 7</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>1488.555583909263</v>
+        <v>1452.20371323302</v>
       </c>
       <c r="D65" t="n">
         <v>15</v>
       </c>
       <c r="E65" t="n">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F65" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G65" t="n">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="H65" t="n">
-        <v>0.008855999029479559</v>
+        <v>0.009717831635639855</v>
       </c>
       <c r="I65" t="n">
-        <v>0.8880262040519229</v>
+        <v>0.880107715724154</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Cromossoma 62</t>
+          <t>Cromossoma 30</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1496.739082566612</v>
+        <v>1463.001962675017</v>
       </c>
       <c r="D66" t="n">
         <v>15</v>
       </c>
       <c r="E66" t="n">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F66" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G66" t="n">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="H66" t="n">
-        <v>0.008613368919082858</v>
+        <v>0.009483667017913594</v>
       </c>
       <c r="I66" t="n">
-        <v>0.8966395729710057</v>
+        <v>0.8895913827420676</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Cromossoma 63</t>
+          <t>Cromossoma 31</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1498.095570644141</v>
+        <v>1475.638097178263</v>
       </c>
       <c r="D67" t="n">
         <v>15</v>
       </c>
       <c r="E67" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F67" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G67" t="n">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="H67" t="n">
-        <v>0.008492053863884508</v>
+        <v>0.00901533778246107</v>
       </c>
       <c r="I67" t="n">
-        <v>0.9051316268348902</v>
+        <v>0.8986067205245287</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Cromossoma 38</t>
+          <t>Cromossoma 26</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>1401.752885585543</v>
+        <v>1477.491985185871</v>
       </c>
       <c r="D68" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E68" t="n">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="F68" t="n">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="G68" t="n">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="H68" t="n">
-        <v>0.008370738808686159</v>
+        <v>0.008781173164734809</v>
       </c>
       <c r="I68" t="n">
-        <v>0.9135023656435763</v>
+        <v>0.9073878936892635</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Cromossoma 68</t>
+          <t>Cromossoma 48</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1513.132811388662</v>
+        <v>1378.9851363771</v>
       </c>
       <c r="D69" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E69" t="n">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="F69" t="n">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="G69" t="n">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="H69" t="n">
-        <v>0.008249423753487807</v>
+        <v>0.008781173164734809</v>
       </c>
       <c r="I69" t="n">
-        <v>0.9217517893970641</v>
+        <v>0.9161690668539983</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>36</v>
+        <v>4</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Cromossoma 36</t>
+          <t>Cromossoma 4</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1516.731159826932</v>
+        <v>1480.022800173836</v>
       </c>
       <c r="D70" t="n">
         <v>15</v>
       </c>
       <c r="E70" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F70" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G70" t="n">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="H70" t="n">
-        <v>0.008128108698289458</v>
+        <v>0.008664090855871678</v>
       </c>
       <c r="I70" t="n">
-        <v>0.9298798980953537</v>
+        <v>0.9248331577098701</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Cromossoma 59</t>
+          <t>Cromossoma 32</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>1549.526412577073</v>
+        <v>1482.060005881544</v>
       </c>
       <c r="D71" t="n">
         <v>15</v>
       </c>
       <c r="E71" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F71" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G71" t="n">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="H71" t="n">
-        <v>0.007764163532694407</v>
+        <v>0.008547008547008548</v>
       </c>
       <c r="I71" t="n">
-        <v>0.937644061628048</v>
+        <v>0.9333801662568786</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Cromossoma 23</t>
+          <t>Cromossoma 81</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>1589.025993295474</v>
+        <v>1496.239189270172</v>
       </c>
       <c r="D72" t="n">
         <v>15</v>
       </c>
       <c r="E72" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F72" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G72" t="n">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="H72" t="n">
-        <v>0.007278903311901007</v>
+        <v>0.007961597002692894</v>
       </c>
       <c r="I72" t="n">
-        <v>0.944922964939949</v>
+        <v>0.9413417632595715</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Cromossoma 70</t>
+          <t>Cromossoma 19</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>1449.024177512655</v>
+        <v>1498.905199353085</v>
       </c>
       <c r="D73" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E73" t="n">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="F73" t="n">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="G73" t="n">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="H73" t="n">
-        <v>0.006308382870314206</v>
+        <v>0.007844514693829763</v>
       </c>
       <c r="I73" t="n">
-        <v>0.9512313478102632</v>
+        <v>0.9491862779534013</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Cromossoma 18</t>
+          <t>Cromossoma 68</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>1449.262626311208</v>
+        <v>1519.718394030406</v>
       </c>
       <c r="D74" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E74" t="n">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="F74" t="n">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="G74" t="n">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="H74" t="n">
-        <v>0.006187067815115856</v>
+        <v>0.007259103149514109</v>
       </c>
       <c r="I74" t="n">
-        <v>0.9574184156253791</v>
+        <v>0.9564453811029153</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>26</v>
+        <v>69</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Cromossoma 26</t>
+          <t>Cromossoma 69</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>1455.576462910018</v>
+        <v>1521.06343330563</v>
       </c>
       <c r="D75" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E75" t="n">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="F75" t="n">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="G75" t="n">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="H75" t="n">
-        <v>0.005823122649520805</v>
+        <v>0.007142020840650977</v>
       </c>
       <c r="I75" t="n">
-        <v>0.9632415382748999</v>
+        <v>0.9635874019435663</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Cromossoma 33</t>
+          <t>Cromossoma 66</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>1456.39743660809</v>
+        <v>1528.018775571936</v>
       </c>
       <c r="D76" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E76" t="n">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="F76" t="n">
-        <v>19</v>
+        <v>58</v>
       </c>
       <c r="G76" t="n">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="H76" t="n">
-        <v>0.005701807594322456</v>
+        <v>0.007024938531787847</v>
       </c>
       <c r="I76" t="n">
-        <v>0.9689433458692224</v>
+        <v>0.9706123404753542</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>49</v>
+        <v>73</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Cromossoma 49</t>
+          <t>Cromossoma 73</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>1424.22143715858</v>
+        <v>1415.397017225511</v>
       </c>
       <c r="D77" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E77" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F77" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G77" t="n">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="H77" t="n">
-        <v>0.004973917263132355</v>
+        <v>0.006205362369745932</v>
       </c>
       <c r="I77" t="n">
-        <v>0.9739172631323547</v>
+        <v>0.9768177028451001</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Cromossoma 65</t>
+          <t>Cromossoma 80</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>1466.882900008875</v>
+        <v>1460.579789035702</v>
       </c>
       <c r="D78" t="n">
         <v>16</v>
       </c>
       <c r="E78" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F78" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G78" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H78" t="n">
-        <v>0.004852602207934004</v>
+        <v>0.004214963119072708</v>
       </c>
       <c r="I78" t="n">
-        <v>0.9787698653402888</v>
+        <v>0.9810326659641727</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Cromossoma 15</t>
+          <t>Cromossoma 75</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>1496.186124859661</v>
+        <v>1469.41905046335</v>
       </c>
       <c r="D79" t="n">
         <v>16</v>
       </c>
       <c r="E79" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F79" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G79" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H79" t="n">
-        <v>0.003882081766347203</v>
+        <v>0.003980798501346447</v>
       </c>
       <c r="I79" t="n">
-        <v>0.9826519471066359</v>
+        <v>0.9850134644655192</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Cromossoma 78</t>
+          <t>Cromossoma 37</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>1507.561679092028</v>
+        <v>1476.736592400702</v>
       </c>
       <c r="D80" t="n">
         <v>16</v>
       </c>
       <c r="E80" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F80" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G80" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H80" t="n">
-        <v>0.003518136600752153</v>
+        <v>0.003512469265893923</v>
       </c>
       <c r="I80" t="n">
-        <v>0.9861700837073881</v>
+        <v>0.9885259337314131</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Cromossoma 54</t>
+          <t>Cromossoma 10</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>1524.406039738066</v>
+        <v>1486.222733802868</v>
       </c>
       <c r="D81" t="n">
         <v>16</v>
       </c>
       <c r="E81" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F81" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G81" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H81" t="n">
-        <v>0.003154191435157103</v>
+        <v>0.00292705772157827</v>
       </c>
       <c r="I81" t="n">
-        <v>0.9893242751425452</v>
+        <v>0.9914529914529914</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Cromossoma 79</t>
+          <t>Cromossoma 1</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>1555.444406965079</v>
+        <v>1489.511405157817</v>
       </c>
       <c r="D82" t="n">
         <v>16</v>
       </c>
       <c r="E82" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F82" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G82" t="n">
         <v>23</v>
       </c>
       <c r="H82" t="n">
-        <v>0.002790246269562052</v>
+        <v>0.002692893103852008</v>
       </c>
       <c r="I82" t="n">
-        <v>0.9921145214121072</v>
+        <v>0.9941458845568434</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Cromossoma 43</t>
+          <t>Cromossoma 17</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>1562.798363432855</v>
+        <v>1504.517832042983</v>
       </c>
       <c r="D83" t="n">
         <v>16</v>
       </c>
       <c r="E83" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F83" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G83" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H83" t="n">
-        <v>0.002668931214363702</v>
+        <v>0.002341646177262616</v>
       </c>
       <c r="I83" t="n">
-        <v>0.9947834526264709</v>
+        <v>0.996487530734106</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Cromossoma 77</t>
+          <t>Cromossoma 45</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>1473.429869140474</v>
+        <v>1514.568056234249</v>
       </c>
       <c r="D84" t="n">
+        <v>16</v>
+      </c>
+      <c r="E84" t="n">
+        <v>5</v>
+      </c>
+      <c r="F84" t="n">
+        <v>12</v>
+      </c>
+      <c r="G84" t="n">
         <v>17</v>
       </c>
-      <c r="E84" t="n">
-        <v>20</v>
-      </c>
-      <c r="F84" t="n">
-        <v>2</v>
-      </c>
-      <c r="G84" t="n">
-        <v>22</v>
-      </c>
       <c r="H84" t="n">
-        <v>0.002668931214363702</v>
+        <v>0.001990399250673223</v>
       </c>
       <c r="I84" t="n">
-        <v>0.9974523838408347</v>
+        <v>0.9984779299847792</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Cromossoma 44</t>
+          <t>Cromossoma 12</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>1580.632485299999</v>
+        <v>1530.369689696431</v>
       </c>
       <c r="D85" t="n">
         <v>16</v>
       </c>
       <c r="E85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F85" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G85" t="n">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H85" t="n">
-        <v>0.002547616159165352</v>
+        <v>0.0015220700152207</v>
       </c>
       <c r="I85" t="n">
         <v>1</v>

</xml_diff>